<commit_message>
Integrate inspectors and add next steps for inspector request - #133
</commit_message>
<xml_diff>
--- a/docassemble/HousingCodeChecklist/data/sources/housing_inspectors.xlsx
+++ b/docassemble/HousingCodeChecklist/data/sources/housing_inspectors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\quinten\docassemble-HousingCodeChecklist\docassemble\HousingCodeChecklist\data\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1777156E-B9DE-4BE3-9B50-3773B0404B6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D096770-FC64-41DB-8CCB-359E082AB9AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="5640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2923" uniqueCount="1890">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2923" uniqueCount="1889">
   <si>
     <t xml:space="preserve">County </t>
   </si>
@@ -4499,21 +4499,6 @@
     <t>Somerville</t>
   </si>
   <si>
-    <t>Health and Human Services Department</t>
-  </si>
-  <si>
-    <t>617-625-6600</t>
-  </si>
-  <si>
-    <t>https://www.somervillema.gov/departments/board-of-health</t>
-  </si>
-  <si>
-    <t>93 Highland Ave</t>
-  </si>
-  <si>
-    <t>02143</t>
-  </si>
-  <si>
     <t>health_webcontact@somervillema.gov</t>
   </si>
   <si>
@@ -5712,6 +5697,18 @@
   </si>
   <si>
     <t>https://www.cambridgema.gov/inspection/contactforms/inspectionalservices</t>
+  </si>
+  <si>
+    <t>https://www.somervillema.gov/departments/isd/health-division</t>
+  </si>
+  <si>
+    <t>1 Franey Rd.</t>
+  </si>
+  <si>
+    <t>02145</t>
+  </si>
+  <si>
+    <t>(617) 625-6600</t>
   </si>
 </sst>
 </file>
@@ -6277,9 +6274,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z980"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K51" sqref="K51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A267" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A274" sqref="A274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
@@ -6301,31 +6298,31 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>1878</v>
+        <v>1873</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1879</v>
+        <v>1874</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1880</v>
+        <v>1875</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1881</v>
+        <v>1876</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1882</v>
+        <v>1877</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>1883</v>
+        <v>1878</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>1884</v>
+        <v>1879</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>2</v>
@@ -8604,14 +8601,14 @@
         <v>53</v>
       </c>
       <c r="D51" t="s">
-        <v>1886</v>
+        <v>1881</v>
       </c>
       <c r="E51" s="18"/>
       <c r="F51" s="25" t="s">
-        <v>1885</v>
+        <v>1880</v>
       </c>
       <c r="G51" t="s">
-        <v>1887</v>
+        <v>1882</v>
       </c>
       <c r="H51" s="17" t="s">
         <v>321</v>
@@ -8620,10 +8617,10 @@
         <v>322</v>
       </c>
       <c r="J51" s="21" t="s">
-        <v>1888</v>
+        <v>1883</v>
       </c>
       <c r="K51" s="22" t="s">
-        <v>1889</v>
+        <v>1884</v>
       </c>
       <c r="L51" s="22"/>
       <c r="M51" s="17"/>
@@ -18587,28 +18584,28 @@
         <v>14</v>
       </c>
       <c r="C274" s="28" t="s">
-        <v>1485</v>
+        <v>53</v>
       </c>
       <c r="D274" s="18" t="s">
-        <v>1486</v>
+        <v>1888</v>
       </c>
       <c r="E274" s="18">
-        <v>4300</v>
+        <v>4331</v>
       </c>
       <c r="F274" s="32" t="s">
-        <v>1487</v>
-      </c>
-      <c r="G274" s="19" t="s">
-        <v>1488</v>
+        <v>1885</v>
+      </c>
+      <c r="G274" t="s">
+        <v>1886</v>
       </c>
       <c r="H274" s="18" t="s">
         <v>1484</v>
       </c>
       <c r="I274" s="21" t="s">
-        <v>1489</v>
+        <v>1887</v>
       </c>
       <c r="J274" s="44" t="s">
-        <v>1490</v>
+        <v>1485</v>
       </c>
       <c r="K274" s="22"/>
       <c r="L274" s="22"/>
@@ -18629,29 +18626,29 @@
     </row>
     <row r="275" spans="1:26" ht="15.75" customHeight="1">
       <c r="A275" s="18" t="s">
-        <v>1491</v>
+        <v>1486</v>
       </c>
       <c r="B275" s="18" t="s">
         <v>62</v>
       </c>
       <c r="C275" s="19" t="s">
-        <v>1492</v>
+        <v>1487</v>
       </c>
       <c r="D275" s="19" t="s">
-        <v>1493</v>
+        <v>1488</v>
       </c>
       <c r="E275" s="18"/>
       <c r="F275" s="32" t="s">
-        <v>1494</v>
+        <v>1489</v>
       </c>
       <c r="G275" s="19" t="s">
-        <v>1495</v>
+        <v>1490</v>
       </c>
       <c r="H275" s="18" t="s">
+        <v>1486</v>
+      </c>
+      <c r="I275" s="21" t="s">
         <v>1491</v>
-      </c>
-      <c r="I275" s="21" t="s">
-        <v>1496</v>
       </c>
       <c r="J275" s="24"/>
       <c r="K275" s="22"/>
@@ -18673,7 +18670,7 @@
     </row>
     <row r="276" spans="1:26" ht="15.75" customHeight="1">
       <c r="A276" s="18" t="s">
-        <v>1497</v>
+        <v>1492</v>
       </c>
       <c r="B276" s="18" t="s">
         <v>62</v>
@@ -18682,23 +18679,23 @@
         <v>63</v>
       </c>
       <c r="D276" s="18" t="s">
-        <v>1498</v>
+        <v>1493</v>
       </c>
       <c r="E276" s="18"/>
       <c r="F276" s="32" t="s">
-        <v>1499</v>
+        <v>1494</v>
       </c>
       <c r="G276" s="19" t="s">
-        <v>1500</v>
+        <v>1495</v>
       </c>
       <c r="H276" s="18" t="s">
+        <v>1492</v>
+      </c>
+      <c r="I276" s="21" t="s">
+        <v>1496</v>
+      </c>
+      <c r="J276" s="44" t="s">
         <v>1497</v>
-      </c>
-      <c r="I276" s="21" t="s">
-        <v>1501</v>
-      </c>
-      <c r="J276" s="44" t="s">
-        <v>1502</v>
       </c>
       <c r="K276" s="22"/>
       <c r="L276" s="22"/>
@@ -18719,29 +18716,29 @@
     </row>
     <row r="277" spans="1:26" ht="15.75" customHeight="1">
       <c r="A277" s="18" t="s">
-        <v>1503</v>
+        <v>1498</v>
       </c>
       <c r="B277" s="18" t="s">
         <v>91</v>
       </c>
       <c r="C277" s="18" t="s">
-        <v>1504</v>
+        <v>1499</v>
       </c>
       <c r="D277" s="18" t="s">
-        <v>1505</v>
+        <v>1500</v>
       </c>
       <c r="E277" s="18"/>
       <c r="F277" s="32" t="s">
-        <v>1506</v>
+        <v>1501</v>
       </c>
       <c r="G277" s="19" t="s">
-        <v>1507</v>
+        <v>1502</v>
       </c>
       <c r="H277" s="18" t="s">
+        <v>1498</v>
+      </c>
+      <c r="I277" s="21" t="s">
         <v>1503</v>
-      </c>
-      <c r="I277" s="21" t="s">
-        <v>1508</v>
       </c>
       <c r="J277" s="24"/>
       <c r="K277" s="22"/>
@@ -18763,7 +18760,7 @@
     </row>
     <row r="278" spans="1:26" ht="15.75" customHeight="1">
       <c r="A278" s="18" t="s">
-        <v>1509</v>
+        <v>1504</v>
       </c>
       <c r="B278" s="18" t="s">
         <v>91</v>
@@ -18772,20 +18769,20 @@
         <v>121</v>
       </c>
       <c r="D278" s="18" t="s">
-        <v>1510</v>
+        <v>1505</v>
       </c>
       <c r="E278" s="18"/>
       <c r="F278" s="32" t="s">
-        <v>1511</v>
+        <v>1506</v>
       </c>
       <c r="G278" s="19" t="s">
-        <v>1512</v>
+        <v>1507</v>
       </c>
       <c r="H278" s="18" t="s">
-        <v>1509</v>
+        <v>1504</v>
       </c>
       <c r="I278" s="21" t="s">
-        <v>1513</v>
+        <v>1508</v>
       </c>
       <c r="J278" s="24"/>
       <c r="K278" s="22"/>
@@ -18807,7 +18804,7 @@
     </row>
     <row r="279" spans="1:26" ht="15.75" customHeight="1">
       <c r="A279" s="18" t="s">
-        <v>1514</v>
+        <v>1509</v>
       </c>
       <c r="B279" s="18" t="s">
         <v>38</v>
@@ -18816,20 +18813,20 @@
         <v>63</v>
       </c>
       <c r="D279" s="28" t="s">
-        <v>1515</v>
+        <v>1510</v>
       </c>
       <c r="E279" s="18"/>
       <c r="F279" s="32" t="s">
-        <v>1516</v>
+        <v>1511</v>
       </c>
       <c r="G279" s="19" t="s">
-        <v>1517</v>
+        <v>1512</v>
       </c>
       <c r="H279" s="18" t="s">
-        <v>1514</v>
+        <v>1509</v>
       </c>
       <c r="I279" s="21" t="s">
-        <v>1518</v>
+        <v>1513</v>
       </c>
       <c r="J279" s="24"/>
       <c r="K279" s="22"/>
@@ -18851,7 +18848,7 @@
     </row>
     <row r="280" spans="1:26" ht="15.75" customHeight="1">
       <c r="A280" s="18" t="s">
-        <v>1519</v>
+        <v>1514</v>
       </c>
       <c r="B280" s="18" t="s">
         <v>91</v>
@@ -18860,22 +18857,22 @@
         <v>63</v>
       </c>
       <c r="D280" s="18" t="s">
-        <v>1520</v>
+        <v>1515</v>
       </c>
       <c r="E280" s="18">
         <v>180</v>
       </c>
       <c r="F280" s="32" t="s">
-        <v>1521</v>
+        <v>1516</v>
       </c>
       <c r="G280" s="19" t="s">
-        <v>1522</v>
+        <v>1517</v>
       </c>
       <c r="H280" s="18" t="s">
-        <v>1519</v>
+        <v>1514</v>
       </c>
       <c r="I280" s="21" t="s">
-        <v>1523</v>
+        <v>1518</v>
       </c>
       <c r="J280" s="24"/>
       <c r="K280" s="22"/>
@@ -18897,7 +18894,7 @@
     </row>
     <row r="281" spans="1:26" ht="15.75" customHeight="1">
       <c r="A281" s="18" t="s">
-        <v>1524</v>
+        <v>1519</v>
       </c>
       <c r="B281" s="18" t="s">
         <v>38</v>
@@ -18906,23 +18903,23 @@
         <v>121</v>
       </c>
       <c r="D281" s="18" t="s">
-        <v>1525</v>
+        <v>1520</v>
       </c>
       <c r="E281" s="18"/>
       <c r="F281" s="32" t="s">
-        <v>1526</v>
+        <v>1521</v>
       </c>
       <c r="G281" s="19" t="s">
-        <v>1527</v>
+        <v>1522</v>
       </c>
       <c r="H281" s="18" t="s">
+        <v>1519</v>
+      </c>
+      <c r="I281" s="21" t="s">
+        <v>1523</v>
+      </c>
+      <c r="J281" s="45" t="s">
         <v>1524</v>
-      </c>
-      <c r="I281" s="21" t="s">
-        <v>1528</v>
-      </c>
-      <c r="J281" s="45" t="s">
-        <v>1529</v>
       </c>
       <c r="K281" s="22"/>
       <c r="L281" s="22"/>
@@ -18943,7 +18940,7 @@
     </row>
     <row r="282" spans="1:26" ht="15.75" customHeight="1">
       <c r="A282" s="18" t="s">
-        <v>1530</v>
+        <v>1525</v>
       </c>
       <c r="B282" s="18" t="s">
         <v>91</v>
@@ -18952,22 +18949,22 @@
         <v>63</v>
       </c>
       <c r="D282" s="19" t="s">
-        <v>1531</v>
+        <v>1526</v>
       </c>
       <c r="E282" s="19">
         <v>2305</v>
       </c>
       <c r="F282" s="32" t="s">
-        <v>1532</v>
+        <v>1527</v>
       </c>
       <c r="G282" s="19" t="s">
-        <v>1533</v>
+        <v>1528</v>
       </c>
       <c r="H282" s="18" t="s">
-        <v>1530</v>
+        <v>1525</v>
       </c>
       <c r="I282" s="21" t="s">
-        <v>1534</v>
+        <v>1529</v>
       </c>
       <c r="J282" s="24"/>
       <c r="K282" s="22"/>
@@ -18989,7 +18986,7 @@
     </row>
     <row r="283" spans="1:26" ht="15.75" customHeight="1">
       <c r="A283" s="18" t="s">
-        <v>1535</v>
+        <v>1530</v>
       </c>
       <c r="B283" s="18" t="s">
         <v>29</v>
@@ -18998,25 +18995,25 @@
         <v>121</v>
       </c>
       <c r="D283" s="19" t="s">
-        <v>1536</v>
+        <v>1531</v>
       </c>
       <c r="E283" s="19">
         <v>314</v>
       </c>
       <c r="F283" s="32" t="s">
-        <v>1537</v>
+        <v>1532</v>
       </c>
       <c r="G283" s="19" t="s">
-        <v>1538</v>
+        <v>1533</v>
       </c>
       <c r="H283" s="18" t="s">
+        <v>1530</v>
+      </c>
+      <c r="I283" s="21" t="s">
+        <v>1534</v>
+      </c>
+      <c r="J283" s="21" t="s">
         <v>1535</v>
-      </c>
-      <c r="I283" s="21" t="s">
-        <v>1539</v>
-      </c>
-      <c r="J283" s="21" t="s">
-        <v>1540</v>
       </c>
       <c r="K283" s="22"/>
       <c r="L283" s="22"/>
@@ -19037,7 +19034,7 @@
     </row>
     <row r="284" spans="1:26" ht="15.75" customHeight="1">
       <c r="A284" s="18" t="s">
-        <v>1541</v>
+        <v>1536</v>
       </c>
       <c r="B284" s="18" t="s">
         <v>14</v>
@@ -19046,20 +19043,20 @@
         <v>63</v>
       </c>
       <c r="D284" s="26" t="s">
-        <v>1542</v>
+        <v>1537</v>
       </c>
       <c r="E284" s="18"/>
       <c r="F284" s="32" t="s">
-        <v>1543</v>
+        <v>1538</v>
       </c>
       <c r="G284" s="19" t="s">
-        <v>1544</v>
+        <v>1539</v>
       </c>
       <c r="H284" s="18" t="s">
-        <v>1541</v>
+        <v>1536</v>
       </c>
       <c r="I284" s="21" t="s">
-        <v>1545</v>
+        <v>1540</v>
       </c>
       <c r="J284" s="24"/>
       <c r="K284" s="22"/>
@@ -19081,7 +19078,7 @@
     </row>
     <row r="285" spans="1:26" ht="15.75" customHeight="1">
       <c r="A285" s="18" t="s">
-        <v>1546</v>
+        <v>1541</v>
       </c>
       <c r="B285" s="18" t="s">
         <v>138</v>
@@ -19090,22 +19087,22 @@
         <v>63</v>
       </c>
       <c r="D285" s="18" t="s">
-        <v>1547</v>
+        <v>1542</v>
       </c>
       <c r="E285" s="19">
         <v>9271</v>
       </c>
       <c r="F285" s="32" t="s">
-        <v>1548</v>
+        <v>1543</v>
       </c>
       <c r="G285" s="19" t="s">
-        <v>1549</v>
+        <v>1544</v>
       </c>
       <c r="H285" s="18" t="s">
-        <v>1546</v>
+        <v>1541</v>
       </c>
       <c r="I285" s="21" t="s">
-        <v>1550</v>
+        <v>1545</v>
       </c>
       <c r="J285" s="24"/>
       <c r="K285" s="22"/>
@@ -19127,7 +19124,7 @@
     </row>
     <row r="286" spans="1:26" ht="15.75" customHeight="1">
       <c r="A286" s="18" t="s">
-        <v>1551</v>
+        <v>1546</v>
       </c>
       <c r="B286" s="18" t="s">
         <v>14</v>
@@ -19136,23 +19133,23 @@
         <v>63</v>
       </c>
       <c r="D286" s="19" t="s">
-        <v>1552</v>
+        <v>1547</v>
       </c>
       <c r="E286" s="18"/>
       <c r="F286" s="32" t="s">
-        <v>1553</v>
+        <v>1548</v>
       </c>
       <c r="G286" s="19" t="s">
-        <v>1554</v>
+        <v>1549</v>
       </c>
       <c r="H286" s="18" t="s">
+        <v>1546</v>
+      </c>
+      <c r="I286" s="21" t="s">
+        <v>1550</v>
+      </c>
+      <c r="J286" s="21" t="s">
         <v>1551</v>
-      </c>
-      <c r="I286" s="21" t="s">
-        <v>1555</v>
-      </c>
-      <c r="J286" s="21" t="s">
-        <v>1556</v>
       </c>
       <c r="K286" s="22"/>
       <c r="L286" s="22"/>
@@ -19173,7 +19170,7 @@
     </row>
     <row r="287" spans="1:26" ht="15.75" customHeight="1">
       <c r="A287" s="18" t="s">
-        <v>1557</v>
+        <v>1552</v>
       </c>
       <c r="B287" s="18" t="s">
         <v>91</v>
@@ -19182,20 +19179,20 @@
         <v>63</v>
       </c>
       <c r="D287" s="18" t="s">
-        <v>1558</v>
+        <v>1553</v>
       </c>
       <c r="E287" s="18"/>
       <c r="F287" s="32" t="s">
-        <v>1559</v>
+        <v>1554</v>
       </c>
       <c r="G287" s="19" t="s">
-        <v>1560</v>
+        <v>1555</v>
       </c>
       <c r="H287" s="18" t="s">
-        <v>1557</v>
+        <v>1552</v>
       </c>
       <c r="I287" s="21" t="s">
-        <v>1561</v>
+        <v>1556</v>
       </c>
       <c r="J287" s="24"/>
       <c r="K287" s="22"/>
@@ -19217,7 +19214,7 @@
     </row>
     <row r="288" spans="1:26" ht="15.75" customHeight="1">
       <c r="A288" s="18" t="s">
-        <v>1562</v>
+        <v>1557</v>
       </c>
       <c r="B288" s="18" t="s">
         <v>14</v>
@@ -19226,23 +19223,23 @@
         <v>63</v>
       </c>
       <c r="D288" s="18" t="s">
-        <v>1563</v>
+        <v>1558</v>
       </c>
       <c r="E288" s="18"/>
       <c r="F288" s="32" t="s">
-        <v>1564</v>
+        <v>1559</v>
       </c>
       <c r="G288" s="19" t="s">
-        <v>1565</v>
+        <v>1560</v>
       </c>
       <c r="H288" s="18" t="s">
+        <v>1557</v>
+      </c>
+      <c r="I288" s="21" t="s">
+        <v>1561</v>
+      </c>
+      <c r="J288" s="21" t="s">
         <v>1562</v>
-      </c>
-      <c r="I288" s="21" t="s">
-        <v>1566</v>
-      </c>
-      <c r="J288" s="21" t="s">
-        <v>1567</v>
       </c>
       <c r="K288" s="22"/>
       <c r="L288" s="22"/>
@@ -19263,31 +19260,31 @@
     </row>
     <row r="289" spans="1:26" ht="15.75" customHeight="1">
       <c r="A289" s="18" t="s">
-        <v>1568</v>
+        <v>1563</v>
       </c>
       <c r="B289" s="18" t="s">
         <v>105</v>
       </c>
       <c r="C289" s="19" t="s">
-        <v>1569</v>
+        <v>1564</v>
       </c>
       <c r="D289" s="18" t="s">
-        <v>1570</v>
+        <v>1565</v>
       </c>
       <c r="E289" s="18">
         <v>6</v>
       </c>
       <c r="F289" s="32" t="s">
-        <v>1571</v>
+        <v>1566</v>
       </c>
       <c r="G289" s="19" t="s">
-        <v>1572</v>
+        <v>1567</v>
       </c>
       <c r="H289" s="18" t="s">
+        <v>1563</v>
+      </c>
+      <c r="I289" s="21" t="s">
         <v>1568</v>
-      </c>
-      <c r="I289" s="21" t="s">
-        <v>1573</v>
       </c>
       <c r="J289" s="24"/>
       <c r="K289" s="22"/>
@@ -19309,7 +19306,7 @@
     </row>
     <row r="290" spans="1:26" ht="15.75" customHeight="1">
       <c r="A290" s="18" t="s">
-        <v>1574</v>
+        <v>1569</v>
       </c>
       <c r="B290" s="18" t="s">
         <v>91</v>
@@ -19318,20 +19315,20 @@
         <v>121</v>
       </c>
       <c r="D290" s="18" t="s">
-        <v>1575</v>
+        <v>1570</v>
       </c>
       <c r="E290" s="18"/>
       <c r="F290" s="32" t="s">
-        <v>1576</v>
+        <v>1571</v>
       </c>
       <c r="G290" s="19" t="s">
-        <v>1577</v>
+        <v>1572</v>
       </c>
       <c r="H290" s="18" t="s">
-        <v>1574</v>
+        <v>1569</v>
       </c>
       <c r="I290" s="21" t="s">
-        <v>1578</v>
+        <v>1573</v>
       </c>
       <c r="J290" s="24"/>
       <c r="K290" s="22"/>
@@ -19353,7 +19350,7 @@
     </row>
     <row r="291" spans="1:26" ht="15.75" customHeight="1">
       <c r="A291" s="18" t="s">
-        <v>1579</v>
+        <v>1574</v>
       </c>
       <c r="B291" s="18" t="s">
         <v>52</v>
@@ -19362,20 +19359,20 @@
         <v>121</v>
       </c>
       <c r="D291" s="18" t="s">
-        <v>1580</v>
+        <v>1575</v>
       </c>
       <c r="E291" s="18"/>
       <c r="F291" s="32" t="s">
-        <v>1581</v>
+        <v>1576</v>
       </c>
       <c r="G291" s="19" t="s">
-        <v>1582</v>
+        <v>1577</v>
       </c>
       <c r="H291" s="18" t="s">
-        <v>1579</v>
+        <v>1574</v>
       </c>
       <c r="I291" s="21" t="s">
-        <v>1583</v>
+        <v>1578</v>
       </c>
       <c r="J291" s="24"/>
       <c r="K291" s="22"/>
@@ -19397,7 +19394,7 @@
     </row>
     <row r="292" spans="1:26" ht="15.75" customHeight="1">
       <c r="A292" s="18" t="s">
-        <v>1584</v>
+        <v>1579</v>
       </c>
       <c r="B292" s="18" t="s">
         <v>22</v>
@@ -19406,22 +19403,22 @@
         <v>63</v>
       </c>
       <c r="D292" s="18" t="s">
-        <v>1585</v>
+        <v>1580</v>
       </c>
       <c r="E292" s="19">
         <v>2</v>
       </c>
       <c r="F292" s="32" t="s">
-        <v>1586</v>
+        <v>1581</v>
       </c>
       <c r="G292" s="19" t="s">
-        <v>1587</v>
+        <v>1582</v>
       </c>
       <c r="H292" s="18" t="s">
-        <v>1584</v>
+        <v>1579</v>
       </c>
       <c r="I292" s="21" t="s">
-        <v>1588</v>
+        <v>1583</v>
       </c>
       <c r="J292" s="24"/>
       <c r="K292" s="22"/>
@@ -19443,7 +19440,7 @@
     </row>
     <row r="293" spans="1:26" ht="15.75" customHeight="1">
       <c r="A293" s="18" t="s">
-        <v>1589</v>
+        <v>1584</v>
       </c>
       <c r="B293" s="18" t="s">
         <v>22</v>
@@ -19452,20 +19449,20 @@
         <v>121</v>
       </c>
       <c r="D293" s="18" t="s">
-        <v>1590</v>
+        <v>1585</v>
       </c>
       <c r="E293" s="18"/>
       <c r="F293" s="32" t="s">
-        <v>1591</v>
+        <v>1586</v>
       </c>
       <c r="G293" s="19" t="s">
-        <v>1592</v>
+        <v>1587</v>
       </c>
       <c r="H293" s="18" t="s">
-        <v>1589</v>
+        <v>1584</v>
       </c>
       <c r="I293" s="21" t="s">
-        <v>1593</v>
+        <v>1588</v>
       </c>
       <c r="J293" s="24"/>
       <c r="K293" s="22"/>
@@ -19487,7 +19484,7 @@
     </row>
     <row r="294" spans="1:26" ht="15.75" customHeight="1">
       <c r="A294" s="18" t="s">
-        <v>1594</v>
+        <v>1589</v>
       </c>
       <c r="B294" s="18" t="s">
         <v>91</v>
@@ -19496,20 +19493,20 @@
         <v>63</v>
       </c>
       <c r="D294" s="18" t="s">
-        <v>1595</v>
+        <v>1590</v>
       </c>
       <c r="E294" s="18"/>
       <c r="F294" s="32" t="s">
-        <v>1596</v>
+        <v>1591</v>
       </c>
       <c r="G294" s="19" t="s">
-        <v>1597</v>
+        <v>1592</v>
       </c>
       <c r="H294" s="18" t="s">
-        <v>1594</v>
+        <v>1589</v>
       </c>
       <c r="I294" s="21" t="s">
-        <v>1598</v>
+        <v>1593</v>
       </c>
       <c r="J294" s="24"/>
       <c r="K294" s="22"/>
@@ -19531,7 +19528,7 @@
     </row>
     <row r="295" spans="1:26" ht="15.75" customHeight="1">
       <c r="A295" s="18" t="s">
-        <v>1599</v>
+        <v>1594</v>
       </c>
       <c r="B295" s="18" t="s">
         <v>14</v>
@@ -19540,20 +19537,20 @@
         <v>121</v>
       </c>
       <c r="D295" s="18" t="s">
-        <v>1600</v>
+        <v>1595</v>
       </c>
       <c r="E295" s="19"/>
       <c r="F295" s="32" t="s">
-        <v>1601</v>
+        <v>1596</v>
       </c>
       <c r="G295" s="19" t="s">
-        <v>1602</v>
+        <v>1597</v>
       </c>
       <c r="H295" s="18" t="s">
-        <v>1599</v>
+        <v>1594</v>
       </c>
       <c r="I295" s="21" t="s">
-        <v>1603</v>
+        <v>1598</v>
       </c>
       <c r="J295" s="24"/>
       <c r="K295" s="22"/>
@@ -19575,7 +19572,7 @@
     </row>
     <row r="296" spans="1:26" ht="15.75" customHeight="1">
       <c r="A296" s="18" t="s">
-        <v>1604</v>
+        <v>1599</v>
       </c>
       <c r="B296" s="18" t="s">
         <v>76</v>
@@ -19584,22 +19581,22 @@
         <v>63</v>
       </c>
       <c r="D296" s="18" t="s">
-        <v>1605</v>
+        <v>1600</v>
       </c>
       <c r="E296" s="19">
         <v>293</v>
       </c>
       <c r="F296" s="32" t="s">
-        <v>1606</v>
+        <v>1601</v>
       </c>
       <c r="G296" s="19" t="s">
-        <v>1607</v>
+        <v>1602</v>
       </c>
       <c r="H296" s="18" t="s">
-        <v>1604</v>
+        <v>1599</v>
       </c>
       <c r="I296" s="21" t="s">
-        <v>1608</v>
+        <v>1603</v>
       </c>
       <c r="J296" s="24"/>
       <c r="K296" s="22"/>
@@ -19621,7 +19618,7 @@
     </row>
     <row r="297" spans="1:26" ht="15.75" customHeight="1">
       <c r="A297" s="18" t="s">
-        <v>1609</v>
+        <v>1604</v>
       </c>
       <c r="B297" s="18" t="s">
         <v>38</v>
@@ -19630,22 +19627,22 @@
         <v>531</v>
       </c>
       <c r="D297" s="19" t="s">
-        <v>1610</v>
+        <v>1605</v>
       </c>
       <c r="E297" s="19">
         <v>127</v>
       </c>
       <c r="F297" s="32" t="s">
-        <v>1611</v>
+        <v>1606</v>
       </c>
       <c r="G297" s="19" t="s">
-        <v>1612</v>
+        <v>1607</v>
       </c>
       <c r="H297" s="18" t="s">
-        <v>1609</v>
+        <v>1604</v>
       </c>
       <c r="I297" s="21" t="s">
-        <v>1613</v>
+        <v>1608</v>
       </c>
       <c r="J297" s="24"/>
       <c r="K297" s="22"/>
@@ -19667,7 +19664,7 @@
     </row>
     <row r="298" spans="1:26" ht="15.75" customHeight="1">
       <c r="A298" s="18" t="s">
-        <v>1614</v>
+        <v>1609</v>
       </c>
       <c r="B298" s="18" t="s">
         <v>52</v>
@@ -19676,23 +19673,23 @@
         <v>7</v>
       </c>
       <c r="D298" s="18" t="s">
-        <v>1615</v>
+        <v>1610</v>
       </c>
       <c r="E298" s="18"/>
       <c r="F298" s="32" t="s">
-        <v>1616</v>
+        <v>1611</v>
       </c>
       <c r="G298" s="19" t="s">
-        <v>1617</v>
+        <v>1612</v>
       </c>
       <c r="H298" s="18" t="s">
+        <v>1609</v>
+      </c>
+      <c r="I298" s="21" t="s">
+        <v>1613</v>
+      </c>
+      <c r="J298" s="21" t="s">
         <v>1614</v>
-      </c>
-      <c r="I298" s="21" t="s">
-        <v>1618</v>
-      </c>
-      <c r="J298" s="21" t="s">
-        <v>1619</v>
       </c>
       <c r="K298" s="22"/>
       <c r="L298" s="22"/>
@@ -19713,29 +19710,29 @@
     </row>
     <row r="299" spans="1:26" ht="15.75" customHeight="1">
       <c r="A299" s="18" t="s">
-        <v>1620</v>
+        <v>1615</v>
       </c>
       <c r="B299" s="18" t="s">
         <v>14</v>
       </c>
       <c r="C299" s="19" t="s">
-        <v>1621</v>
+        <v>1616</v>
       </c>
       <c r="D299" s="18" t="s">
-        <v>1622</v>
+        <v>1617</v>
       </c>
       <c r="E299" s="18"/>
       <c r="F299" s="32" t="s">
-        <v>1623</v>
+        <v>1618</v>
       </c>
       <c r="G299" s="19" t="s">
-        <v>1624</v>
+        <v>1619</v>
       </c>
       <c r="H299" s="18" t="s">
+        <v>1615</v>
+      </c>
+      <c r="I299" s="21" t="s">
         <v>1620</v>
-      </c>
-      <c r="I299" s="21" t="s">
-        <v>1625</v>
       </c>
       <c r="J299" s="24"/>
       <c r="K299" s="22"/>
@@ -19757,7 +19754,7 @@
     </row>
     <row r="300" spans="1:26" ht="15.75" customHeight="1">
       <c r="A300" s="18" t="s">
-        <v>1626</v>
+        <v>1621</v>
       </c>
       <c r="B300" s="18" t="s">
         <v>151</v>
@@ -19766,20 +19763,20 @@
         <v>121</v>
       </c>
       <c r="D300" s="19" t="s">
-        <v>1627</v>
+        <v>1622</v>
       </c>
       <c r="E300" s="18"/>
       <c r="F300" s="32" t="s">
-        <v>1628</v>
+        <v>1623</v>
       </c>
       <c r="G300" s="19" t="s">
-        <v>1629</v>
+        <v>1624</v>
       </c>
       <c r="H300" s="18" t="s">
-        <v>1626</v>
+        <v>1621</v>
       </c>
       <c r="I300" s="21" t="s">
-        <v>1630</v>
+        <v>1625</v>
       </c>
       <c r="J300" s="24"/>
       <c r="K300" s="22"/>
@@ -19801,7 +19798,7 @@
     </row>
     <row r="301" spans="1:26" ht="15.75" customHeight="1">
       <c r="A301" s="18" t="s">
-        <v>1631</v>
+        <v>1626</v>
       </c>
       <c r="B301" s="18" t="s">
         <v>14</v>
@@ -19810,25 +19807,25 @@
         <v>63</v>
       </c>
       <c r="D301" s="18" t="s">
-        <v>1632</v>
+        <v>1627</v>
       </c>
       <c r="E301" s="18">
         <v>118</v>
       </c>
       <c r="F301" s="32" t="s">
-        <v>1633</v>
+        <v>1628</v>
       </c>
       <c r="G301" s="19" t="s">
-        <v>1634</v>
+        <v>1629</v>
       </c>
       <c r="H301" s="18" t="s">
+        <v>1626</v>
+      </c>
+      <c r="I301" s="21" t="s">
+        <v>1630</v>
+      </c>
+      <c r="J301" s="44" t="s">
         <v>1631</v>
-      </c>
-      <c r="I301" s="21" t="s">
-        <v>1635</v>
-      </c>
-      <c r="J301" s="44" t="s">
-        <v>1636</v>
       </c>
       <c r="K301" s="22"/>
       <c r="L301" s="22"/>
@@ -19849,7 +19846,7 @@
     </row>
     <row r="302" spans="1:26" ht="15.75" customHeight="1">
       <c r="A302" s="18" t="s">
-        <v>1637</v>
+        <v>1632</v>
       </c>
       <c r="B302" s="18" t="s">
         <v>29</v>
@@ -19858,20 +19855,20 @@
         <v>63</v>
       </c>
       <c r="D302" s="18" t="s">
-        <v>1638</v>
+        <v>1633</v>
       </c>
       <c r="E302" s="18"/>
       <c r="F302" s="32" t="s">
-        <v>1639</v>
+        <v>1634</v>
       </c>
       <c r="G302" s="19" t="s">
-        <v>1640</v>
+        <v>1635</v>
       </c>
       <c r="H302" s="18" t="s">
-        <v>1637</v>
+        <v>1632</v>
       </c>
       <c r="I302" s="21" t="s">
-        <v>1641</v>
+        <v>1636</v>
       </c>
       <c r="J302" s="24"/>
       <c r="K302" s="22"/>
@@ -19893,7 +19890,7 @@
     </row>
     <row r="303" spans="1:26" ht="15.75" customHeight="1">
       <c r="A303" s="18" t="s">
-        <v>1642</v>
+        <v>1637</v>
       </c>
       <c r="B303" s="18" t="s">
         <v>91</v>
@@ -19902,20 +19899,20 @@
         <v>63</v>
       </c>
       <c r="D303" s="18" t="s">
-        <v>1643</v>
+        <v>1638</v>
       </c>
       <c r="E303" s="18"/>
       <c r="F303" s="32" t="s">
-        <v>1644</v>
+        <v>1639</v>
       </c>
       <c r="G303" s="19" t="s">
         <v>1264</v>
       </c>
       <c r="H303" s="18" t="s">
-        <v>1642</v>
+        <v>1637</v>
       </c>
       <c r="I303" s="21" t="s">
-        <v>1645</v>
+        <v>1640</v>
       </c>
       <c r="J303" s="24"/>
       <c r="K303" s="22"/>
@@ -19937,7 +19934,7 @@
     </row>
     <row r="304" spans="1:26" ht="15.75" customHeight="1">
       <c r="A304" s="18" t="s">
-        <v>1646</v>
+        <v>1641</v>
       </c>
       <c r="B304" s="18" t="s">
         <v>91</v>
@@ -19946,22 +19943,22 @@
         <v>63</v>
       </c>
       <c r="D304" s="26" t="s">
-        <v>1647</v>
+        <v>1642</v>
       </c>
       <c r="E304" s="19">
         <v>8</v>
       </c>
       <c r="F304" s="32" t="s">
-        <v>1648</v>
+        <v>1643</v>
       </c>
       <c r="G304" s="19" t="s">
-        <v>1649</v>
+        <v>1644</v>
       </c>
       <c r="H304" s="18" t="s">
-        <v>1646</v>
+        <v>1641</v>
       </c>
       <c r="I304" s="21" t="s">
-        <v>1650</v>
+        <v>1645</v>
       </c>
       <c r="J304" s="24"/>
       <c r="K304" s="22"/>
@@ -19983,7 +19980,7 @@
     </row>
     <row r="305" spans="1:26" ht="15.75" customHeight="1">
       <c r="A305" s="18" t="s">
-        <v>1651</v>
+        <v>1646</v>
       </c>
       <c r="B305" s="18" t="s">
         <v>14</v>
@@ -19992,20 +19989,20 @@
         <v>1141</v>
       </c>
       <c r="D305" s="18" t="s">
-        <v>1652</v>
+        <v>1647</v>
       </c>
       <c r="E305" s="18"/>
       <c r="F305" s="32" t="s">
-        <v>1653</v>
+        <v>1648</v>
       </c>
       <c r="G305" s="19" t="s">
-        <v>1654</v>
+        <v>1649</v>
       </c>
       <c r="H305" s="18" t="s">
-        <v>1651</v>
+        <v>1646</v>
       </c>
       <c r="I305" s="21" t="s">
-        <v>1655</v>
+        <v>1650</v>
       </c>
       <c r="J305" s="24"/>
       <c r="K305" s="22"/>
@@ -20027,7 +20024,7 @@
     </row>
     <row r="306" spans="1:26" ht="15.75" customHeight="1">
       <c r="A306" s="18" t="s">
-        <v>1656</v>
+        <v>1651</v>
       </c>
       <c r="B306" s="18" t="s">
         <v>38</v>
@@ -20036,22 +20033,22 @@
         <v>63</v>
       </c>
       <c r="D306" s="18" t="s">
-        <v>1657</v>
+        <v>1652</v>
       </c>
       <c r="E306" s="18">
         <v>105</v>
       </c>
       <c r="F306" s="32" t="s">
-        <v>1658</v>
+        <v>1653</v>
       </c>
       <c r="G306" s="19" t="s">
-        <v>1659</v>
+        <v>1654</v>
       </c>
       <c r="H306" s="18" t="s">
-        <v>1656</v>
+        <v>1651</v>
       </c>
       <c r="I306" s="21" t="s">
-        <v>1660</v>
+        <v>1655</v>
       </c>
       <c r="J306" s="24"/>
       <c r="K306" s="22"/>
@@ -20073,7 +20070,7 @@
     </row>
     <row r="307" spans="1:26" ht="15.75" customHeight="1">
       <c r="A307" s="18" t="s">
-        <v>1661</v>
+        <v>1656</v>
       </c>
       <c r="B307" s="18" t="s">
         <v>138</v>
@@ -20082,20 +20079,20 @@
         <v>63</v>
       </c>
       <c r="D307" s="18" t="s">
-        <v>1662</v>
+        <v>1657</v>
       </c>
       <c r="E307" s="18"/>
       <c r="F307" s="32" t="s">
-        <v>1663</v>
+        <v>1658</v>
       </c>
       <c r="G307" s="19" t="s">
-        <v>1664</v>
+        <v>1659</v>
       </c>
       <c r="H307" s="18" t="s">
-        <v>1661</v>
+        <v>1656</v>
       </c>
       <c r="I307" s="21" t="s">
-        <v>1665</v>
+        <v>1660</v>
       </c>
       <c r="J307" s="24"/>
       <c r="K307" s="22"/>
@@ -20117,7 +20114,7 @@
     </row>
     <row r="308" spans="1:26" ht="15.75" customHeight="1">
       <c r="A308" s="18" t="s">
-        <v>1666</v>
+        <v>1661</v>
       </c>
       <c r="B308" s="18" t="s">
         <v>14</v>
@@ -20126,20 +20123,20 @@
         <v>121</v>
       </c>
       <c r="D308" s="18" t="s">
-        <v>1667</v>
+        <v>1662</v>
       </c>
       <c r="E308" s="18"/>
       <c r="F308" s="32" t="s">
-        <v>1668</v>
+        <v>1663</v>
       </c>
       <c r="G308" s="19" t="s">
-        <v>1669</v>
+        <v>1664</v>
       </c>
       <c r="H308" s="18" t="s">
-        <v>1666</v>
+        <v>1661</v>
       </c>
       <c r="I308" s="21" t="s">
-        <v>1670</v>
+        <v>1665</v>
       </c>
       <c r="J308" s="24"/>
       <c r="K308" s="22"/>
@@ -20161,7 +20158,7 @@
     </row>
     <row r="309" spans="1:26" ht="15.75" customHeight="1">
       <c r="A309" s="18" t="s">
-        <v>1671</v>
+        <v>1666</v>
       </c>
       <c r="B309" s="18" t="s">
         <v>62</v>
@@ -20176,16 +20173,16 @@
         <v>116</v>
       </c>
       <c r="F309" s="32" t="s">
-        <v>1672</v>
+        <v>1667</v>
       </c>
       <c r="G309" s="19" t="s">
-        <v>1673</v>
+        <v>1668</v>
       </c>
       <c r="H309" s="18" t="s">
-        <v>1671</v>
+        <v>1666</v>
       </c>
       <c r="I309" s="21" t="s">
-        <v>1674</v>
+        <v>1669</v>
       </c>
       <c r="J309" s="24"/>
       <c r="K309" s="22"/>
@@ -20207,7 +20204,7 @@
     </row>
     <row r="310" spans="1:26" ht="15.75" customHeight="1">
       <c r="A310" s="18" t="s">
-        <v>1675</v>
+        <v>1670</v>
       </c>
       <c r="B310" s="18" t="s">
         <v>6</v>
@@ -20216,22 +20213,22 @@
         <v>121</v>
       </c>
       <c r="D310" s="26" t="s">
-        <v>1676</v>
+        <v>1671</v>
       </c>
       <c r="E310" s="18">
         <v>3196</v>
       </c>
       <c r="F310" s="32" t="s">
-        <v>1677</v>
+        <v>1672</v>
       </c>
       <c r="G310" s="19" t="s">
-        <v>1678</v>
+        <v>1673</v>
       </c>
       <c r="H310" s="18" t="s">
-        <v>1675</v>
+        <v>1670</v>
       </c>
       <c r="I310" s="21" t="s">
-        <v>1679</v>
+        <v>1674</v>
       </c>
       <c r="J310" s="24"/>
       <c r="K310" s="22"/>
@@ -20253,7 +20250,7 @@
     </row>
     <row r="311" spans="1:26" ht="15.75" customHeight="1">
       <c r="A311" s="46" t="s">
-        <v>1680</v>
+        <v>1675</v>
       </c>
       <c r="B311" s="18" t="s">
         <v>91</v>
@@ -20262,22 +20259,22 @@
         <v>63</v>
       </c>
       <c r="D311" s="18" t="s">
-        <v>1681</v>
+        <v>1676</v>
       </c>
       <c r="E311" s="18">
         <v>112</v>
       </c>
       <c r="F311" s="32" t="s">
-        <v>1682</v>
+        <v>1677</v>
       </c>
       <c r="G311" s="19" t="s">
-        <v>1683</v>
+        <v>1678</v>
       </c>
       <c r="H311" s="18" t="s">
-        <v>1680</v>
+        <v>1675</v>
       </c>
       <c r="I311" s="21" t="s">
-        <v>1684</v>
+        <v>1679</v>
       </c>
       <c r="J311" s="24"/>
       <c r="K311" s="22"/>
@@ -20299,7 +20296,7 @@
     </row>
     <row r="312" spans="1:26" ht="15.75" customHeight="1">
       <c r="A312" s="18" t="s">
-        <v>1685</v>
+        <v>1680</v>
       </c>
       <c r="B312" s="18" t="s">
         <v>105</v>
@@ -20308,20 +20305,20 @@
         <v>63</v>
       </c>
       <c r="D312" s="18" t="s">
-        <v>1686</v>
+        <v>1681</v>
       </c>
       <c r="E312" s="18"/>
       <c r="F312" s="32" t="s">
-        <v>1687</v>
+        <v>1682</v>
       </c>
       <c r="G312" s="19" t="s">
-        <v>1688</v>
+        <v>1683</v>
       </c>
       <c r="H312" s="18" t="s">
-        <v>1685</v>
+        <v>1680</v>
       </c>
       <c r="I312" s="21" t="s">
-        <v>1689</v>
+        <v>1684</v>
       </c>
       <c r="J312" s="24"/>
       <c r="K312" s="22"/>
@@ -20343,7 +20340,7 @@
     </row>
     <row r="313" spans="1:26" ht="15.75" customHeight="1">
       <c r="A313" s="18" t="s">
-        <v>1690</v>
+        <v>1685</v>
       </c>
       <c r="B313" s="18" t="s">
         <v>29</v>
@@ -20358,13 +20355,13 @@
         <v>60</v>
       </c>
       <c r="F313" s="32" t="s">
-        <v>1691</v>
+        <v>1686</v>
       </c>
       <c r="G313" s="19" t="s">
-        <v>1692</v>
+        <v>1687</v>
       </c>
       <c r="H313" s="18" t="s">
-        <v>1690</v>
+        <v>1685</v>
       </c>
       <c r="I313" s="21" t="s">
         <v>169</v>
@@ -20389,7 +20386,7 @@
     </row>
     <row r="314" spans="1:26" ht="15.75" customHeight="1">
       <c r="A314" s="18" t="s">
-        <v>1693</v>
+        <v>1688</v>
       </c>
       <c r="B314" s="18" t="s">
         <v>14</v>
@@ -20398,20 +20395,20 @@
         <v>121</v>
       </c>
       <c r="D314" s="18" t="s">
-        <v>1694</v>
+        <v>1689</v>
       </c>
       <c r="E314" s="18"/>
       <c r="F314" s="32" t="s">
-        <v>1695</v>
+        <v>1690</v>
       </c>
       <c r="G314" s="19" t="s">
-        <v>1696</v>
+        <v>1691</v>
       </c>
       <c r="H314" s="18" t="s">
-        <v>1693</v>
+        <v>1688</v>
       </c>
       <c r="I314" s="21" t="s">
-        <v>1697</v>
+        <v>1692</v>
       </c>
       <c r="J314" s="24"/>
       <c r="K314" s="22"/>
@@ -20433,7 +20430,7 @@
     </row>
     <row r="315" spans="1:26" ht="15.75" customHeight="1">
       <c r="A315" s="18" t="s">
-        <v>1698</v>
+        <v>1693</v>
       </c>
       <c r="B315" s="18" t="s">
         <v>14</v>
@@ -20442,23 +20439,23 @@
         <v>63</v>
       </c>
       <c r="D315" s="19" t="s">
-        <v>1699</v>
+        <v>1694</v>
       </c>
       <c r="E315" s="18"/>
       <c r="F315" s="32" t="s">
-        <v>1700</v>
+        <v>1695</v>
       </c>
       <c r="G315" s="19" t="s">
-        <v>1701</v>
+        <v>1696</v>
       </c>
       <c r="H315" s="18" t="s">
+        <v>1693</v>
+      </c>
+      <c r="I315" s="21" t="s">
+        <v>1697</v>
+      </c>
+      <c r="J315" s="21" t="s">
         <v>1698</v>
-      </c>
-      <c r="I315" s="21" t="s">
-        <v>1702</v>
-      </c>
-      <c r="J315" s="21" t="s">
-        <v>1703</v>
       </c>
       <c r="K315" s="22"/>
       <c r="L315" s="22"/>
@@ -20479,7 +20476,7 @@
     </row>
     <row r="316" spans="1:26" ht="15.75" customHeight="1">
       <c r="A316" s="18" t="s">
-        <v>1704</v>
+        <v>1699</v>
       </c>
       <c r="B316" s="18" t="s">
         <v>91</v>
@@ -20488,22 +20485,22 @@
         <v>63</v>
       </c>
       <c r="D316" s="18" t="s">
-        <v>1705</v>
+        <v>1700</v>
       </c>
       <c r="E316" s="18">
         <v>4002</v>
       </c>
       <c r="F316" s="32" t="s">
-        <v>1706</v>
+        <v>1701</v>
       </c>
       <c r="G316" s="19" t="s">
-        <v>1707</v>
+        <v>1702</v>
       </c>
       <c r="H316" s="18" t="s">
-        <v>1704</v>
+        <v>1699</v>
       </c>
       <c r="I316" s="21" t="s">
-        <v>1708</v>
+        <v>1703</v>
       </c>
       <c r="J316" s="24"/>
       <c r="K316" s="22"/>
@@ -20525,7 +20522,7 @@
     </row>
     <row r="317" spans="1:26" ht="15.75" customHeight="1">
       <c r="A317" s="18" t="s">
-        <v>1709</v>
+        <v>1704</v>
       </c>
       <c r="B317" s="18" t="s">
         <v>138</v>
@@ -20534,20 +20531,20 @@
         <v>63</v>
       </c>
       <c r="D317" s="18" t="s">
-        <v>1710</v>
+        <v>1705</v>
       </c>
       <c r="E317" s="18"/>
       <c r="F317" s="32" t="s">
-        <v>1711</v>
+        <v>1706</v>
       </c>
       <c r="G317" s="19" t="s">
-        <v>1712</v>
+        <v>1707</v>
       </c>
       <c r="H317" s="18" t="s">
-        <v>1709</v>
+        <v>1704</v>
       </c>
       <c r="I317" s="21" t="s">
-        <v>1713</v>
+        <v>1708</v>
       </c>
       <c r="J317" s="24"/>
       <c r="K317" s="22"/>
@@ -20569,7 +20566,7 @@
     </row>
     <row r="318" spans="1:26" ht="15.75" customHeight="1">
       <c r="A318" s="18" t="s">
-        <v>1714</v>
+        <v>1709</v>
       </c>
       <c r="B318" s="18" t="s">
         <v>151</v>
@@ -20578,20 +20575,20 @@
         <v>121</v>
       </c>
       <c r="D318" s="18" t="s">
-        <v>1715</v>
+        <v>1710</v>
       </c>
       <c r="E318" s="18"/>
       <c r="F318" s="32" t="s">
-        <v>1716</v>
+        <v>1711</v>
       </c>
       <c r="G318" s="19" t="s">
-        <v>1717</v>
+        <v>1712</v>
       </c>
       <c r="H318" s="18" t="s">
-        <v>1714</v>
+        <v>1709</v>
       </c>
       <c r="I318" s="21" t="s">
-        <v>1718</v>
+        <v>1713</v>
       </c>
       <c r="J318" s="24"/>
       <c r="K318" s="22"/>
@@ -20613,7 +20610,7 @@
     </row>
     <row r="319" spans="1:26" ht="15.75" customHeight="1">
       <c r="A319" s="18" t="s">
-        <v>1719</v>
+        <v>1714</v>
       </c>
       <c r="B319" s="18" t="s">
         <v>105</v>
@@ -20622,25 +20619,25 @@
         <v>63</v>
       </c>
       <c r="D319" s="18" t="s">
-        <v>1720</v>
+        <v>1715</v>
       </c>
       <c r="E319" s="18">
         <v>106</v>
       </c>
       <c r="F319" s="32" t="s">
-        <v>1721</v>
+        <v>1716</v>
       </c>
       <c r="G319" s="19" t="s">
-        <v>1722</v>
+        <v>1717</v>
       </c>
       <c r="H319" s="18" t="s">
+        <v>1714</v>
+      </c>
+      <c r="I319" s="21" t="s">
+        <v>1718</v>
+      </c>
+      <c r="J319" s="21" t="s">
         <v>1719</v>
-      </c>
-      <c r="I319" s="21" t="s">
-        <v>1723</v>
-      </c>
-      <c r="J319" s="21" t="s">
-        <v>1724</v>
       </c>
       <c r="K319" s="22"/>
       <c r="L319" s="22"/>
@@ -20661,7 +20658,7 @@
     </row>
     <row r="320" spans="1:26" ht="15.75" customHeight="1">
       <c r="A320" s="18" t="s">
-        <v>1725</v>
+        <v>1720</v>
       </c>
       <c r="B320" s="18" t="s">
         <v>52</v>
@@ -20670,22 +20667,22 @@
         <v>63</v>
       </c>
       <c r="D320" s="26" t="s">
-        <v>1726</v>
+        <v>1721</v>
       </c>
       <c r="E320" s="18">
         <v>4</v>
       </c>
       <c r="F320" s="32" t="s">
-        <v>1727</v>
+        <v>1722</v>
       </c>
       <c r="G320" s="19" t="s">
-        <v>1728</v>
+        <v>1723</v>
       </c>
       <c r="H320" s="18" t="s">
-        <v>1725</v>
+        <v>1720</v>
       </c>
       <c r="I320" s="21" t="s">
-        <v>1729</v>
+        <v>1724</v>
       </c>
       <c r="J320" s="24"/>
       <c r="K320" s="22"/>
@@ -20707,7 +20704,7 @@
     </row>
     <row r="321" spans="1:26" ht="15.75" customHeight="1">
       <c r="A321" s="18" t="s">
-        <v>1730</v>
+        <v>1725</v>
       </c>
       <c r="B321" s="18" t="s">
         <v>91</v>
@@ -20716,20 +20713,20 @@
         <v>121</v>
       </c>
       <c r="D321" s="18" t="s">
-        <v>1731</v>
+        <v>1726</v>
       </c>
       <c r="E321" s="18"/>
       <c r="F321" s="23" t="s">
-        <v>1732</v>
+        <v>1727</v>
       </c>
       <c r="G321" s="19" t="s">
-        <v>1733</v>
+        <v>1728</v>
       </c>
       <c r="H321" s="18" t="s">
-        <v>1730</v>
+        <v>1725</v>
       </c>
       <c r="I321" s="21" t="s">
-        <v>1734</v>
+        <v>1729</v>
       </c>
       <c r="J321" s="24"/>
       <c r="K321" s="22"/>
@@ -20751,7 +20748,7 @@
     </row>
     <row r="322" spans="1:26" ht="15.75" customHeight="1">
       <c r="A322" s="18" t="s">
-        <v>1735</v>
+        <v>1730</v>
       </c>
       <c r="B322" s="18" t="s">
         <v>6</v>
@@ -20760,20 +20757,20 @@
         <v>63</v>
       </c>
       <c r="D322" s="18" t="s">
-        <v>1736</v>
+        <v>1731</v>
       </c>
       <c r="E322" s="18"/>
       <c r="F322" s="32" t="s">
-        <v>1737</v>
+        <v>1732</v>
       </c>
       <c r="G322" s="19" t="s">
-        <v>1738</v>
+        <v>1733</v>
       </c>
       <c r="H322" s="18" t="s">
-        <v>1735</v>
+        <v>1730</v>
       </c>
       <c r="I322" s="21" t="s">
-        <v>1739</v>
+        <v>1734</v>
       </c>
       <c r="J322" s="24"/>
       <c r="K322" s="22"/>
@@ -20795,7 +20792,7 @@
     </row>
     <row r="323" spans="1:26" ht="15.75" customHeight="1">
       <c r="A323" s="18" t="s">
-        <v>1740</v>
+        <v>1735</v>
       </c>
       <c r="B323" s="18" t="s">
         <v>91</v>
@@ -20804,25 +20801,25 @@
         <v>63</v>
       </c>
       <c r="D323" s="18" t="s">
-        <v>1741</v>
+        <v>1736</v>
       </c>
       <c r="E323" s="18">
         <v>310</v>
       </c>
       <c r="F323" s="32" t="s">
-        <v>1742</v>
+        <v>1737</v>
       </c>
       <c r="G323" s="19" t="s">
-        <v>1743</v>
+        <v>1738</v>
       </c>
       <c r="H323" s="18" t="s">
+        <v>1735</v>
+      </c>
+      <c r="I323" s="21" t="s">
+        <v>1739</v>
+      </c>
+      <c r="J323" s="21" t="s">
         <v>1740</v>
-      </c>
-      <c r="I323" s="21" t="s">
-        <v>1744</v>
-      </c>
-      <c r="J323" s="21" t="s">
-        <v>1745</v>
       </c>
       <c r="K323" s="22"/>
       <c r="L323" s="22"/>
@@ -20843,7 +20840,7 @@
     </row>
     <row r="324" spans="1:26" ht="15.75" customHeight="1">
       <c r="A324" s="18" t="s">
-        <v>1746</v>
+        <v>1741</v>
       </c>
       <c r="B324" s="18" t="s">
         <v>52</v>
@@ -20852,20 +20849,20 @@
         <v>63</v>
       </c>
       <c r="D324" s="18" t="s">
-        <v>1747</v>
+        <v>1742</v>
       </c>
       <c r="E324" s="18"/>
       <c r="F324" s="32" t="s">
-        <v>1748</v>
+        <v>1743</v>
       </c>
       <c r="G324" s="19" t="s">
-        <v>1749</v>
+        <v>1744</v>
       </c>
       <c r="H324" s="18" t="s">
-        <v>1746</v>
+        <v>1741</v>
       </c>
       <c r="I324" s="21" t="s">
-        <v>1750</v>
+        <v>1745</v>
       </c>
       <c r="J324" s="24"/>
       <c r="K324" s="22"/>
@@ -20887,7 +20884,7 @@
     </row>
     <row r="325" spans="1:26" ht="15.75" customHeight="1">
       <c r="A325" s="18" t="s">
-        <v>1751</v>
+        <v>1746</v>
       </c>
       <c r="B325" s="18" t="s">
         <v>38</v>
@@ -20896,20 +20893,20 @@
         <v>63</v>
       </c>
       <c r="D325" s="18" t="s">
-        <v>1752</v>
+        <v>1747</v>
       </c>
       <c r="E325" s="47"/>
       <c r="F325" s="32" t="s">
-        <v>1753</v>
+        <v>1748</v>
       </c>
       <c r="G325" s="19" t="s">
-        <v>1754</v>
+        <v>1749</v>
       </c>
       <c r="H325" s="18" t="s">
-        <v>1751</v>
+        <v>1746</v>
       </c>
       <c r="I325" s="21" t="s">
-        <v>1755</v>
+        <v>1750</v>
       </c>
       <c r="J325" s="24"/>
       <c r="K325" s="22"/>
@@ -20931,7 +20928,7 @@
     </row>
     <row r="326" spans="1:26" ht="15.75" customHeight="1">
       <c r="A326" s="18" t="s">
-        <v>1756</v>
+        <v>1751</v>
       </c>
       <c r="B326" s="18" t="s">
         <v>29</v>
@@ -20940,22 +20937,22 @@
         <v>63</v>
       </c>
       <c r="D326" s="18" t="s">
-        <v>1757</v>
+        <v>1752</v>
       </c>
       <c r="E326" s="18">
         <v>314</v>
       </c>
       <c r="F326" s="32" t="s">
-        <v>1758</v>
+        <v>1753</v>
       </c>
       <c r="G326" s="19" t="s">
-        <v>1538</v>
+        <v>1533</v>
       </c>
       <c r="H326" s="18" t="s">
-        <v>1756</v>
+        <v>1751</v>
       </c>
       <c r="I326" s="21" t="s">
-        <v>1539</v>
+        <v>1534</v>
       </c>
       <c r="J326" s="24"/>
       <c r="K326" s="22"/>
@@ -20977,7 +20974,7 @@
     </row>
     <row r="327" spans="1:26" ht="15.75" customHeight="1">
       <c r="A327" s="18" t="s">
-        <v>1759</v>
+        <v>1754</v>
       </c>
       <c r="B327" s="18" t="s">
         <v>76</v>
@@ -20986,23 +20983,23 @@
         <v>63</v>
       </c>
       <c r="D327" s="18" t="s">
-        <v>1760</v>
+        <v>1755</v>
       </c>
       <c r="E327" s="18"/>
       <c r="F327" s="32" t="s">
-        <v>1761</v>
+        <v>1756</v>
       </c>
       <c r="G327" s="19" t="s">
-        <v>1762</v>
+        <v>1757</v>
       </c>
       <c r="H327" s="18" t="s">
-        <v>1759</v>
+        <v>1754</v>
       </c>
       <c r="I327" s="21" t="s">
-        <v>1608</v>
+        <v>1603</v>
       </c>
       <c r="J327" s="21" t="s">
-        <v>1763</v>
+        <v>1758</v>
       </c>
       <c r="K327" s="22"/>
       <c r="L327" s="22"/>
@@ -21023,7 +21020,7 @@
     </row>
     <row r="328" spans="1:26" ht="15.75" customHeight="1">
       <c r="A328" s="18" t="s">
-        <v>1764</v>
+        <v>1759</v>
       </c>
       <c r="B328" s="18" t="s">
         <v>91</v>
@@ -21032,20 +21029,20 @@
         <v>63</v>
       </c>
       <c r="D328" s="18" t="s">
-        <v>1765</v>
+        <v>1760</v>
       </c>
       <c r="E328" s="18"/>
       <c r="F328" s="32" t="s">
-        <v>1766</v>
+        <v>1761</v>
       </c>
       <c r="G328" s="19" t="s">
-        <v>1767</v>
+        <v>1762</v>
       </c>
       <c r="H328" s="18" t="s">
-        <v>1764</v>
+        <v>1759</v>
       </c>
       <c r="I328" s="21" t="s">
-        <v>1768</v>
+        <v>1763</v>
       </c>
       <c r="J328" s="24"/>
       <c r="K328" s="22"/>
@@ -21067,26 +21064,26 @@
     </row>
     <row r="329" spans="1:26" ht="15.75" customHeight="1">
       <c r="A329" s="18" t="s">
-        <v>1769</v>
+        <v>1764</v>
       </c>
       <c r="B329" s="18" t="s">
         <v>38</v>
       </c>
       <c r="C329" s="28" t="s">
-        <v>1770</v>
+        <v>1765</v>
       </c>
       <c r="D329" s="18" t="s">
-        <v>1771</v>
+        <v>1766</v>
       </c>
       <c r="E329" s="18"/>
       <c r="F329" s="32" t="s">
-        <v>1772</v>
+        <v>1767</v>
       </c>
       <c r="G329" s="19" t="s">
-        <v>1773</v>
+        <v>1768</v>
       </c>
       <c r="H329" s="18" t="s">
-        <v>1769</v>
+        <v>1764</v>
       </c>
       <c r="I329" s="21" t="s">
         <v>1081</v>
@@ -21111,7 +21108,7 @@
     </row>
     <row r="330" spans="1:26" ht="15.75" customHeight="1">
       <c r="A330" s="18" t="s">
-        <v>1774</v>
+        <v>1769</v>
       </c>
       <c r="B330" s="18" t="s">
         <v>14</v>
@@ -21120,20 +21117,20 @@
         <v>63</v>
       </c>
       <c r="D330" s="26" t="s">
-        <v>1775</v>
+        <v>1770</v>
       </c>
       <c r="E330" s="18"/>
       <c r="F330" s="32" t="s">
-        <v>1776</v>
+        <v>1771</v>
       </c>
       <c r="G330" s="19" t="s">
-        <v>1777</v>
+        <v>1772</v>
       </c>
       <c r="H330" s="18" t="s">
-        <v>1774</v>
+        <v>1769</v>
       </c>
       <c r="I330" s="21" t="s">
-        <v>1778</v>
+        <v>1773</v>
       </c>
       <c r="J330" s="24"/>
       <c r="K330" s="22"/>
@@ -21155,7 +21152,7 @@
     </row>
     <row r="331" spans="1:26" ht="15.75" customHeight="1">
       <c r="A331" s="46" t="s">
-        <v>1779</v>
+        <v>1774</v>
       </c>
       <c r="B331" s="18" t="s">
         <v>62</v>
@@ -21164,20 +21161,20 @@
         <v>63</v>
       </c>
       <c r="D331" s="18" t="s">
-        <v>1780</v>
+        <v>1775</v>
       </c>
       <c r="E331" s="18"/>
       <c r="F331" s="32" t="s">
-        <v>1781</v>
+        <v>1776</v>
       </c>
       <c r="G331" s="19" t="s">
-        <v>1782</v>
+        <v>1777</v>
       </c>
       <c r="H331" s="18" t="s">
-        <v>1779</v>
+        <v>1774</v>
       </c>
       <c r="I331" s="21" t="s">
-        <v>1783</v>
+        <v>1778</v>
       </c>
       <c r="J331" s="24"/>
       <c r="K331" s="22"/>
@@ -21199,7 +21196,7 @@
     </row>
     <row r="332" spans="1:26" ht="15.75" customHeight="1">
       <c r="A332" s="18" t="s">
-        <v>1784</v>
+        <v>1779</v>
       </c>
       <c r="B332" s="18" t="s">
         <v>91</v>
@@ -21208,20 +21205,20 @@
         <v>121</v>
       </c>
       <c r="D332" s="18" t="s">
-        <v>1785</v>
+        <v>1780</v>
       </c>
       <c r="E332" s="18"/>
       <c r="F332" s="32" t="s">
-        <v>1786</v>
+        <v>1781</v>
       </c>
       <c r="G332" s="19" t="s">
-        <v>1787</v>
+        <v>1782</v>
       </c>
       <c r="H332" s="18" t="s">
-        <v>1784</v>
+        <v>1779</v>
       </c>
       <c r="I332" s="21" t="s">
-        <v>1788</v>
+        <v>1783</v>
       </c>
       <c r="J332" s="24"/>
       <c r="K332" s="22"/>
@@ -21243,7 +21240,7 @@
     </row>
     <row r="333" spans="1:26" ht="15.75" customHeight="1">
       <c r="A333" s="18" t="s">
-        <v>1789</v>
+        <v>1784</v>
       </c>
       <c r="B333" s="18" t="s">
         <v>14</v>
@@ -21252,20 +21249,20 @@
         <v>63</v>
       </c>
       <c r="D333" s="18" t="s">
-        <v>1790</v>
+        <v>1785</v>
       </c>
       <c r="E333" s="18"/>
       <c r="F333" s="32" t="s">
-        <v>1791</v>
+        <v>1786</v>
       </c>
       <c r="G333" s="19" t="s">
-        <v>1792</v>
+        <v>1787</v>
       </c>
       <c r="H333" s="18" t="s">
-        <v>1789</v>
+        <v>1784</v>
       </c>
       <c r="I333" s="21" t="s">
-        <v>1793</v>
+        <v>1788</v>
       </c>
       <c r="J333" s="24"/>
       <c r="K333" s="22"/>
@@ -21287,7 +21284,7 @@
     </row>
     <row r="334" spans="1:26" ht="15.75" customHeight="1">
       <c r="A334" s="18" t="s">
-        <v>1794</v>
+        <v>1789</v>
       </c>
       <c r="B334" s="18" t="s">
         <v>22</v>
@@ -21296,20 +21293,20 @@
         <v>63</v>
       </c>
       <c r="D334" s="18" t="s">
-        <v>1795</v>
+        <v>1790</v>
       </c>
       <c r="E334" s="18"/>
       <c r="F334" s="32" t="s">
-        <v>1796</v>
+        <v>1791</v>
       </c>
       <c r="G334" s="19" t="s">
-        <v>1797</v>
+        <v>1792</v>
       </c>
       <c r="H334" s="18" t="s">
-        <v>1794</v>
+        <v>1789</v>
       </c>
       <c r="I334" s="21" t="s">
-        <v>1798</v>
+        <v>1793</v>
       </c>
       <c r="J334" s="24"/>
       <c r="K334" s="22"/>
@@ -21331,7 +21328,7 @@
     </row>
     <row r="335" spans="1:26" ht="15.75" customHeight="1">
       <c r="A335" s="18" t="s">
-        <v>1799</v>
+        <v>1794</v>
       </c>
       <c r="B335" s="18" t="s">
         <v>138</v>
@@ -21340,20 +21337,20 @@
         <v>264</v>
       </c>
       <c r="D335" s="18" t="s">
-        <v>1800</v>
+        <v>1795</v>
       </c>
       <c r="E335" s="18"/>
       <c r="F335" s="32" t="s">
-        <v>1801</v>
+        <v>1796</v>
       </c>
       <c r="G335" s="19" t="s">
-        <v>1802</v>
+        <v>1797</v>
       </c>
       <c r="H335" s="18" t="s">
-        <v>1799</v>
+        <v>1794</v>
       </c>
       <c r="I335" s="21" t="s">
-        <v>1803</v>
+        <v>1798</v>
       </c>
       <c r="J335" s="24"/>
       <c r="K335" s="22"/>
@@ -21375,7 +21372,7 @@
     </row>
     <row r="336" spans="1:26" ht="15.75" customHeight="1">
       <c r="A336" s="18" t="s">
-        <v>1804</v>
+        <v>1799</v>
       </c>
       <c r="B336" s="18" t="s">
         <v>138</v>
@@ -21384,20 +21381,20 @@
         <v>121</v>
       </c>
       <c r="D336" s="18" t="s">
-        <v>1805</v>
+        <v>1800</v>
       </c>
       <c r="E336" s="18"/>
       <c r="F336" s="32" t="s">
-        <v>1806</v>
+        <v>1801</v>
       </c>
       <c r="G336" s="19" t="s">
-        <v>1807</v>
+        <v>1802</v>
       </c>
       <c r="H336" s="18" t="s">
-        <v>1804</v>
+        <v>1799</v>
       </c>
       <c r="I336" s="21" t="s">
-        <v>1808</v>
+        <v>1803</v>
       </c>
       <c r="J336" s="24"/>
       <c r="K336" s="22"/>
@@ -21419,7 +21416,7 @@
     </row>
     <row r="337" spans="1:26" ht="15.75" customHeight="1">
       <c r="A337" s="18" t="s">
-        <v>1809</v>
+        <v>1804</v>
       </c>
       <c r="B337" s="18" t="s">
         <v>105</v>
@@ -21428,20 +21425,20 @@
         <v>63</v>
       </c>
       <c r="D337" s="18" t="s">
-        <v>1810</v>
+        <v>1805</v>
       </c>
       <c r="E337" s="18"/>
       <c r="F337" s="32" t="s">
-        <v>1811</v>
+        <v>1806</v>
       </c>
       <c r="G337" s="19" t="s">
-        <v>1782</v>
+        <v>1777</v>
       </c>
       <c r="H337" s="18" t="s">
-        <v>1809</v>
+        <v>1804</v>
       </c>
       <c r="I337" s="21" t="s">
-        <v>1783</v>
+        <v>1778</v>
       </c>
       <c r="J337" s="24"/>
       <c r="K337" s="22"/>
@@ -21463,7 +21460,7 @@
     </row>
     <row r="338" spans="1:26" ht="15.75" customHeight="1">
       <c r="A338" s="18" t="s">
-        <v>1812</v>
+        <v>1807</v>
       </c>
       <c r="B338" s="18" t="s">
         <v>6</v>
@@ -21472,20 +21469,20 @@
         <v>63</v>
       </c>
       <c r="D338" s="18" t="s">
-        <v>1813</v>
+        <v>1808</v>
       </c>
       <c r="E338" s="18"/>
       <c r="F338" s="32" t="s">
-        <v>1814</v>
+        <v>1809</v>
       </c>
       <c r="G338" s="19" t="s">
-        <v>1815</v>
+        <v>1810</v>
       </c>
       <c r="H338" s="18" t="s">
-        <v>1812</v>
+        <v>1807</v>
       </c>
       <c r="I338" s="21" t="s">
-        <v>1816</v>
+        <v>1811</v>
       </c>
       <c r="J338" s="24"/>
       <c r="K338" s="22"/>
@@ -21507,7 +21504,7 @@
     </row>
     <row r="339" spans="1:26" ht="15.75" customHeight="1">
       <c r="A339" s="18" t="s">
-        <v>1817</v>
+        <v>1812</v>
       </c>
       <c r="B339" s="18" t="s">
         <v>38</v>
@@ -21516,17 +21513,17 @@
         <v>121</v>
       </c>
       <c r="D339" s="18" t="s">
-        <v>1818</v>
+        <v>1813</v>
       </c>
       <c r="E339" s="18">
         <v>101</v>
       </c>
       <c r="F339" s="32" t="s">
-        <v>1819</v>
+        <v>1814</v>
       </c>
       <c r="G339" s="18"/>
       <c r="H339" s="18" t="s">
-        <v>1817</v>
+        <v>1812</v>
       </c>
       <c r="I339" s="24"/>
       <c r="J339" s="24"/>
@@ -21549,7 +21546,7 @@
     </row>
     <row r="340" spans="1:26" ht="15.75" customHeight="1">
       <c r="A340" s="46" t="s">
-        <v>1820</v>
+        <v>1815</v>
       </c>
       <c r="B340" s="18" t="s">
         <v>62</v>
@@ -21558,20 +21555,20 @@
         <v>63</v>
       </c>
       <c r="D340" s="33" t="s">
-        <v>1810</v>
+        <v>1805</v>
       </c>
       <c r="E340" s="18"/>
       <c r="F340" s="32" t="s">
-        <v>1821</v>
+        <v>1816</v>
       </c>
       <c r="G340" s="19" t="s">
-        <v>1782</v>
+        <v>1777</v>
       </c>
       <c r="H340" s="18" t="s">
-        <v>1820</v>
+        <v>1815</v>
       </c>
       <c r="I340" s="21" t="s">
-        <v>1783</v>
+        <v>1778</v>
       </c>
       <c r="J340" s="24"/>
       <c r="K340" s="22"/>
@@ -21593,7 +21590,7 @@
     </row>
     <row r="341" spans="1:26" ht="15.75" customHeight="1">
       <c r="A341" s="18" t="s">
-        <v>1822</v>
+        <v>1817</v>
       </c>
       <c r="B341" s="18" t="s">
         <v>29</v>
@@ -21602,20 +21599,20 @@
         <v>63</v>
       </c>
       <c r="D341" s="18" t="s">
-        <v>1823</v>
+        <v>1818</v>
       </c>
       <c r="E341" s="18"/>
       <c r="F341" s="32" t="s">
-        <v>1824</v>
+        <v>1819</v>
       </c>
       <c r="G341" s="19" t="s">
-        <v>1825</v>
+        <v>1820</v>
       </c>
       <c r="H341" s="18" t="s">
-        <v>1822</v>
+        <v>1817</v>
       </c>
       <c r="I341" s="21" t="s">
-        <v>1826</v>
+        <v>1821</v>
       </c>
       <c r="J341" s="24"/>
       <c r="K341" s="22"/>
@@ -21637,7 +21634,7 @@
     </row>
     <row r="342" spans="1:26" ht="15.75" customHeight="1">
       <c r="A342" s="18" t="s">
-        <v>1827</v>
+        <v>1822</v>
       </c>
       <c r="B342" s="18" t="s">
         <v>14</v>
@@ -21646,20 +21643,20 @@
         <v>63</v>
       </c>
       <c r="D342" s="18" t="s">
-        <v>1828</v>
+        <v>1823</v>
       </c>
       <c r="E342" s="18"/>
       <c r="F342" s="32" t="s">
-        <v>1829</v>
+        <v>1824</v>
       </c>
       <c r="G342" s="19" t="s">
-        <v>1830</v>
+        <v>1825</v>
       </c>
       <c r="H342" s="18" t="s">
-        <v>1827</v>
+        <v>1822</v>
       </c>
       <c r="I342" s="21" t="s">
-        <v>1831</v>
+        <v>1826</v>
       </c>
       <c r="J342" s="24"/>
       <c r="K342" s="22"/>
@@ -21681,7 +21678,7 @@
     </row>
     <row r="343" spans="1:26" ht="15.75" customHeight="1">
       <c r="A343" s="18" t="s">
-        <v>1832</v>
+        <v>1827</v>
       </c>
       <c r="B343" s="18" t="s">
         <v>91</v>
@@ -21690,20 +21687,20 @@
         <v>63</v>
       </c>
       <c r="D343" s="18" t="s">
-        <v>1833</v>
+        <v>1828</v>
       </c>
       <c r="E343" s="18"/>
       <c r="F343" s="32" t="s">
-        <v>1834</v>
+        <v>1829</v>
       </c>
       <c r="G343" s="19" t="s">
-        <v>1835</v>
+        <v>1830</v>
       </c>
       <c r="H343" s="18" t="s">
-        <v>1832</v>
+        <v>1827</v>
       </c>
       <c r="I343" s="21" t="s">
-        <v>1836</v>
+        <v>1831</v>
       </c>
       <c r="J343" s="24"/>
       <c r="K343" s="22"/>
@@ -21725,29 +21722,29 @@
     </row>
     <row r="344" spans="1:26" ht="15.75" customHeight="1">
       <c r="A344" s="18" t="s">
-        <v>1837</v>
+        <v>1832</v>
       </c>
       <c r="B344" s="18" t="s">
         <v>14</v>
       </c>
       <c r="C344" s="19" t="s">
-        <v>1838</v>
+        <v>1833</v>
       </c>
       <c r="D344" s="18" t="s">
-        <v>1839</v>
+        <v>1834</v>
       </c>
       <c r="E344" s="18"/>
       <c r="F344" s="32" t="s">
-        <v>1840</v>
+        <v>1835</v>
       </c>
       <c r="G344" s="19" t="s">
-        <v>1841</v>
+        <v>1836</v>
       </c>
       <c r="H344" s="18" t="s">
+        <v>1832</v>
+      </c>
+      <c r="I344" s="21" t="s">
         <v>1837</v>
-      </c>
-      <c r="I344" s="21" t="s">
-        <v>1842</v>
       </c>
       <c r="J344" s="24"/>
       <c r="K344" s="22"/>
@@ -21769,7 +21766,7 @@
     </row>
     <row r="345" spans="1:26" ht="15.75" customHeight="1">
       <c r="A345" s="18" t="s">
-        <v>1843</v>
+        <v>1838</v>
       </c>
       <c r="B345" s="18" t="s">
         <v>29</v>
@@ -21778,22 +21775,22 @@
         <v>63</v>
       </c>
       <c r="D345" s="18" t="s">
-        <v>1844</v>
+        <v>1839</v>
       </c>
       <c r="E345" s="18">
         <v>7</v>
       </c>
       <c r="F345" s="32" t="s">
-        <v>1845</v>
+        <v>1840</v>
       </c>
       <c r="G345" s="19" t="s">
-        <v>1846</v>
+        <v>1841</v>
       </c>
       <c r="H345" s="18" t="s">
-        <v>1843</v>
+        <v>1838</v>
       </c>
       <c r="I345" s="21" t="s">
-        <v>1847</v>
+        <v>1842</v>
       </c>
       <c r="J345" s="24"/>
       <c r="K345" s="22"/>
@@ -21815,7 +21812,7 @@
     </row>
     <row r="346" spans="1:26" ht="15.75" customHeight="1">
       <c r="A346" s="18" t="s">
-        <v>1848</v>
+        <v>1843</v>
       </c>
       <c r="B346" s="18" t="s">
         <v>236</v>
@@ -21824,22 +21821,22 @@
         <v>121</v>
       </c>
       <c r="D346" s="18" t="s">
-        <v>1849</v>
+        <v>1844</v>
       </c>
       <c r="E346" s="18">
         <v>1061</v>
       </c>
       <c r="F346" s="32" t="s">
-        <v>1850</v>
+        <v>1845</v>
       </c>
       <c r="G346" s="19" t="s">
-        <v>1851</v>
+        <v>1846</v>
       </c>
       <c r="H346" s="18" t="s">
-        <v>1848</v>
+        <v>1843</v>
       </c>
       <c r="I346" s="21" t="s">
-        <v>1852</v>
+        <v>1847</v>
       </c>
       <c r="J346" s="24"/>
       <c r="K346" s="22"/>
@@ -21861,7 +21858,7 @@
     </row>
     <row r="347" spans="1:26" ht="15.75" customHeight="1">
       <c r="A347" s="18" t="s">
-        <v>1853</v>
+        <v>1848</v>
       </c>
       <c r="B347" s="18" t="s">
         <v>14</v>
@@ -21870,20 +21867,20 @@
         <v>121</v>
       </c>
       <c r="D347" s="28" t="s">
-        <v>1854</v>
+        <v>1849</v>
       </c>
       <c r="E347" s="18"/>
       <c r="F347" s="32" t="s">
-        <v>1855</v>
+        <v>1850</v>
       </c>
       <c r="G347" s="19" t="s">
-        <v>1856</v>
+        <v>1851</v>
       </c>
       <c r="H347" s="18" t="s">
-        <v>1853</v>
+        <v>1848</v>
       </c>
       <c r="I347" s="21" t="s">
-        <v>1857</v>
+        <v>1852</v>
       </c>
       <c r="J347" s="24"/>
       <c r="K347" s="22"/>
@@ -21914,23 +21911,23 @@
         <v>1141</v>
       </c>
       <c r="D348" s="19" t="s">
-        <v>1858</v>
+        <v>1853</v>
       </c>
       <c r="E348" s="18"/>
       <c r="F348" s="32" t="s">
-        <v>1859</v>
+        <v>1854</v>
       </c>
       <c r="G348" s="19" t="s">
-        <v>1860</v>
+        <v>1855</v>
       </c>
       <c r="H348" s="18" t="s">
         <v>91</v>
       </c>
       <c r="I348" s="21" t="s">
-        <v>1861</v>
+        <v>1856</v>
       </c>
       <c r="K348" s="48" t="s">
-        <v>1862</v>
+        <v>1857</v>
       </c>
       <c r="L348" s="49"/>
       <c r="M348" s="17"/>
@@ -21950,7 +21947,7 @@
     </row>
     <row r="349" spans="1:26" ht="15.75" customHeight="1">
       <c r="A349" s="18" t="s">
-        <v>1863</v>
+        <v>1858</v>
       </c>
       <c r="B349" s="18" t="s">
         <v>62</v>
@@ -21959,22 +21956,22 @@
         <v>63</v>
       </c>
       <c r="D349" s="18" t="s">
-        <v>1864</v>
+        <v>1859</v>
       </c>
       <c r="E349" s="18">
         <v>106</v>
       </c>
       <c r="F349" s="32" t="s">
-        <v>1865</v>
+        <v>1860</v>
       </c>
       <c r="G349" s="19" t="s">
-        <v>1866</v>
+        <v>1861</v>
       </c>
       <c r="H349" s="18" t="s">
-        <v>1863</v>
+        <v>1858</v>
       </c>
       <c r="I349" s="21" t="s">
-        <v>1867</v>
+        <v>1862</v>
       </c>
       <c r="J349" s="24"/>
       <c r="K349" s="22"/>
@@ -21996,7 +21993,7 @@
     </row>
     <row r="350" spans="1:26" ht="15.75" customHeight="1">
       <c r="A350" s="18" t="s">
-        <v>1868</v>
+        <v>1863</v>
       </c>
       <c r="B350" s="18" t="s">
         <v>138</v>
@@ -22005,20 +22002,20 @@
         <v>63</v>
       </c>
       <c r="D350" s="26" t="s">
-        <v>1869</v>
+        <v>1864</v>
       </c>
       <c r="E350" s="18"/>
       <c r="F350" s="32" t="s">
-        <v>1870</v>
+        <v>1865</v>
       </c>
       <c r="G350" s="19" t="s">
-        <v>1871</v>
+        <v>1866</v>
       </c>
       <c r="H350" s="18" t="s">
-        <v>1868</v>
+        <v>1863</v>
       </c>
       <c r="I350" s="21" t="s">
-        <v>1872</v>
+        <v>1867</v>
       </c>
       <c r="J350" s="24"/>
       <c r="K350" s="22"/>
@@ -22040,7 +22037,7 @@
     </row>
     <row r="351" spans="1:26" ht="15.75" customHeight="1">
       <c r="A351" s="18" t="s">
-        <v>1873</v>
+        <v>1868</v>
       </c>
       <c r="B351" s="18" t="s">
         <v>151</v>
@@ -22049,22 +22046,22 @@
         <v>63</v>
       </c>
       <c r="D351" s="18" t="s">
-        <v>1874</v>
+        <v>1869</v>
       </c>
       <c r="E351" s="18">
         <v>1241</v>
       </c>
       <c r="F351" s="32" t="s">
-        <v>1875</v>
+        <v>1870</v>
       </c>
       <c r="G351" s="19" t="s">
-        <v>1876</v>
+        <v>1871</v>
       </c>
       <c r="H351" s="18" t="s">
-        <v>1873</v>
+        <v>1868</v>
       </c>
       <c r="I351" s="21" t="s">
-        <v>1877</v>
+        <v>1872</v>
       </c>
       <c r="J351" s="24"/>
       <c r="K351" s="22"/>
@@ -39980,86 +39977,85 @@
     <hyperlink ref="F272" r:id="rId279" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
     <hyperlink ref="F273" r:id="rId280" xr:uid="{00000000-0004-0000-0000-000018010000}"/>
     <hyperlink ref="J273" r:id="rId281" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
-    <hyperlink ref="F274" r:id="rId282" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
-    <hyperlink ref="F275" r:id="rId283" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
-    <hyperlink ref="F276" r:id="rId284" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
-    <hyperlink ref="F277" r:id="rId285" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
-    <hyperlink ref="F278" r:id="rId286" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
-    <hyperlink ref="F279" r:id="rId287" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
-    <hyperlink ref="F280" r:id="rId288" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
-    <hyperlink ref="F281" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
-    <hyperlink ref="J281" r:id="rId290" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
-    <hyperlink ref="F282" r:id="rId291" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
-    <hyperlink ref="F283" r:id="rId292" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
-    <hyperlink ref="F284" r:id="rId293" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
-    <hyperlink ref="F285" r:id="rId294" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
-    <hyperlink ref="F286" r:id="rId295" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
-    <hyperlink ref="F287" r:id="rId296" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
-    <hyperlink ref="F288" r:id="rId297" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
-    <hyperlink ref="F289" r:id="rId298" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
-    <hyperlink ref="F290" r:id="rId299" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
-    <hyperlink ref="F291" r:id="rId300" xr:uid="{00000000-0004-0000-0000-00002C010000}"/>
-    <hyperlink ref="F292" r:id="rId301" xr:uid="{00000000-0004-0000-0000-00002D010000}"/>
-    <hyperlink ref="F293" r:id="rId302" xr:uid="{00000000-0004-0000-0000-00002E010000}"/>
-    <hyperlink ref="F294" r:id="rId303" xr:uid="{00000000-0004-0000-0000-00002F010000}"/>
-    <hyperlink ref="F295" r:id="rId304" xr:uid="{00000000-0004-0000-0000-000030010000}"/>
-    <hyperlink ref="F296" r:id="rId305" xr:uid="{00000000-0004-0000-0000-000031010000}"/>
-    <hyperlink ref="F297" r:id="rId306" xr:uid="{00000000-0004-0000-0000-000032010000}"/>
-    <hyperlink ref="F298" r:id="rId307" xr:uid="{00000000-0004-0000-0000-000033010000}"/>
-    <hyperlink ref="F299" r:id="rId308" xr:uid="{00000000-0004-0000-0000-000034010000}"/>
-    <hyperlink ref="F300" r:id="rId309" xr:uid="{00000000-0004-0000-0000-000035010000}"/>
-    <hyperlink ref="F301" r:id="rId310" xr:uid="{00000000-0004-0000-0000-000036010000}"/>
-    <hyperlink ref="F302" r:id="rId311" xr:uid="{00000000-0004-0000-0000-000037010000}"/>
-    <hyperlink ref="F303" r:id="rId312" xr:uid="{00000000-0004-0000-0000-000038010000}"/>
-    <hyperlink ref="F304" r:id="rId313" xr:uid="{00000000-0004-0000-0000-000039010000}"/>
-    <hyperlink ref="F305" r:id="rId314" xr:uid="{00000000-0004-0000-0000-00003A010000}"/>
-    <hyperlink ref="F306" r:id="rId315" xr:uid="{00000000-0004-0000-0000-00003B010000}"/>
-    <hyperlink ref="F307" r:id="rId316" xr:uid="{00000000-0004-0000-0000-00003C010000}"/>
-    <hyperlink ref="F308" r:id="rId317" xr:uid="{00000000-0004-0000-0000-00003D010000}"/>
-    <hyperlink ref="F309" r:id="rId318" xr:uid="{00000000-0004-0000-0000-00003E010000}"/>
-    <hyperlink ref="F310" r:id="rId319" xr:uid="{00000000-0004-0000-0000-00003F010000}"/>
-    <hyperlink ref="F311" r:id="rId320" xr:uid="{00000000-0004-0000-0000-000040010000}"/>
-    <hyperlink ref="F312" r:id="rId321" xr:uid="{00000000-0004-0000-0000-000041010000}"/>
-    <hyperlink ref="F313" r:id="rId322" xr:uid="{00000000-0004-0000-0000-000042010000}"/>
-    <hyperlink ref="F314" r:id="rId323" xr:uid="{00000000-0004-0000-0000-000043010000}"/>
-    <hyperlink ref="F315" r:id="rId324" xr:uid="{00000000-0004-0000-0000-000044010000}"/>
-    <hyperlink ref="F316" r:id="rId325" xr:uid="{00000000-0004-0000-0000-000045010000}"/>
-    <hyperlink ref="F317" r:id="rId326" xr:uid="{00000000-0004-0000-0000-000046010000}"/>
-    <hyperlink ref="F318" r:id="rId327" xr:uid="{00000000-0004-0000-0000-000047010000}"/>
-    <hyperlink ref="F319" r:id="rId328" xr:uid="{00000000-0004-0000-0000-000048010000}"/>
-    <hyperlink ref="F320" r:id="rId329" xr:uid="{00000000-0004-0000-0000-000049010000}"/>
-    <hyperlink ref="F321" r:id="rId330" xr:uid="{00000000-0004-0000-0000-00004A010000}"/>
-    <hyperlink ref="F322" r:id="rId331" xr:uid="{00000000-0004-0000-0000-00004B010000}"/>
-    <hyperlink ref="F323" r:id="rId332" xr:uid="{00000000-0004-0000-0000-00004C010000}"/>
-    <hyperlink ref="F324" r:id="rId333" xr:uid="{00000000-0004-0000-0000-00004D010000}"/>
-    <hyperlink ref="F325" r:id="rId334" xr:uid="{00000000-0004-0000-0000-00004E010000}"/>
-    <hyperlink ref="F326" r:id="rId335" xr:uid="{00000000-0004-0000-0000-00004F010000}"/>
-    <hyperlink ref="F327" r:id="rId336" xr:uid="{00000000-0004-0000-0000-000050010000}"/>
-    <hyperlink ref="F328" r:id="rId337" xr:uid="{00000000-0004-0000-0000-000051010000}"/>
-    <hyperlink ref="F329" r:id="rId338" xr:uid="{00000000-0004-0000-0000-000052010000}"/>
-    <hyperlink ref="F330" r:id="rId339" xr:uid="{00000000-0004-0000-0000-000053010000}"/>
-    <hyperlink ref="F331" r:id="rId340" xr:uid="{00000000-0004-0000-0000-000054010000}"/>
-    <hyperlink ref="F332" r:id="rId341" xr:uid="{00000000-0004-0000-0000-000055010000}"/>
-    <hyperlink ref="F333" r:id="rId342" xr:uid="{00000000-0004-0000-0000-000056010000}"/>
-    <hyperlink ref="F334" r:id="rId343" xr:uid="{00000000-0004-0000-0000-000057010000}"/>
-    <hyperlink ref="F335" r:id="rId344" xr:uid="{00000000-0004-0000-0000-000058010000}"/>
-    <hyperlink ref="F336" r:id="rId345" xr:uid="{00000000-0004-0000-0000-000059010000}"/>
-    <hyperlink ref="F337" r:id="rId346" xr:uid="{00000000-0004-0000-0000-00005A010000}"/>
-    <hyperlink ref="F338" r:id="rId347" xr:uid="{00000000-0004-0000-0000-00005B010000}"/>
-    <hyperlink ref="F339" r:id="rId348" xr:uid="{00000000-0004-0000-0000-00005C010000}"/>
-    <hyperlink ref="F340" r:id="rId349" xr:uid="{00000000-0004-0000-0000-00005D010000}"/>
-    <hyperlink ref="F341" r:id="rId350" xr:uid="{00000000-0004-0000-0000-00005E010000}"/>
-    <hyperlink ref="F342" r:id="rId351" xr:uid="{00000000-0004-0000-0000-00005F010000}"/>
-    <hyperlink ref="F343" r:id="rId352" xr:uid="{00000000-0004-0000-0000-000060010000}"/>
-    <hyperlink ref="F344" r:id="rId353" xr:uid="{00000000-0004-0000-0000-000061010000}"/>
-    <hyperlink ref="F345" r:id="rId354" xr:uid="{00000000-0004-0000-0000-000062010000}"/>
-    <hyperlink ref="F346" r:id="rId355" xr:uid="{00000000-0004-0000-0000-000063010000}"/>
-    <hyperlink ref="F347" r:id="rId356" xr:uid="{00000000-0004-0000-0000-000064010000}"/>
-    <hyperlink ref="F348" r:id="rId357" xr:uid="{00000000-0004-0000-0000-000065010000}"/>
-    <hyperlink ref="K348" r:id="rId358" xr:uid="{00000000-0004-0000-0000-000066010000}"/>
-    <hyperlink ref="F349" r:id="rId359" xr:uid="{00000000-0004-0000-0000-000067010000}"/>
-    <hyperlink ref="F350" r:id="rId360" xr:uid="{00000000-0004-0000-0000-000068010000}"/>
-    <hyperlink ref="F351" r:id="rId361" xr:uid="{00000000-0004-0000-0000-000069010000}"/>
+    <hyperlink ref="F275" r:id="rId282" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
+    <hyperlink ref="F276" r:id="rId283" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
+    <hyperlink ref="F277" r:id="rId284" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
+    <hyperlink ref="F278" r:id="rId285" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
+    <hyperlink ref="F279" r:id="rId286" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
+    <hyperlink ref="F280" r:id="rId287" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
+    <hyperlink ref="F281" r:id="rId288" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
+    <hyperlink ref="J281" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
+    <hyperlink ref="F282" r:id="rId290" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
+    <hyperlink ref="F283" r:id="rId291" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
+    <hyperlink ref="F284" r:id="rId292" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
+    <hyperlink ref="F285" r:id="rId293" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
+    <hyperlink ref="F286" r:id="rId294" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
+    <hyperlink ref="F287" r:id="rId295" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
+    <hyperlink ref="F288" r:id="rId296" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
+    <hyperlink ref="F289" r:id="rId297" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
+    <hyperlink ref="F290" r:id="rId298" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
+    <hyperlink ref="F291" r:id="rId299" xr:uid="{00000000-0004-0000-0000-00002C010000}"/>
+    <hyperlink ref="F292" r:id="rId300" xr:uid="{00000000-0004-0000-0000-00002D010000}"/>
+    <hyperlink ref="F293" r:id="rId301" xr:uid="{00000000-0004-0000-0000-00002E010000}"/>
+    <hyperlink ref="F294" r:id="rId302" xr:uid="{00000000-0004-0000-0000-00002F010000}"/>
+    <hyperlink ref="F295" r:id="rId303" xr:uid="{00000000-0004-0000-0000-000030010000}"/>
+    <hyperlink ref="F296" r:id="rId304" xr:uid="{00000000-0004-0000-0000-000031010000}"/>
+    <hyperlink ref="F297" r:id="rId305" xr:uid="{00000000-0004-0000-0000-000032010000}"/>
+    <hyperlink ref="F298" r:id="rId306" xr:uid="{00000000-0004-0000-0000-000033010000}"/>
+    <hyperlink ref="F299" r:id="rId307" xr:uid="{00000000-0004-0000-0000-000034010000}"/>
+    <hyperlink ref="F300" r:id="rId308" xr:uid="{00000000-0004-0000-0000-000035010000}"/>
+    <hyperlink ref="F301" r:id="rId309" xr:uid="{00000000-0004-0000-0000-000036010000}"/>
+    <hyperlink ref="F302" r:id="rId310" xr:uid="{00000000-0004-0000-0000-000037010000}"/>
+    <hyperlink ref="F303" r:id="rId311" xr:uid="{00000000-0004-0000-0000-000038010000}"/>
+    <hyperlink ref="F304" r:id="rId312" xr:uid="{00000000-0004-0000-0000-000039010000}"/>
+    <hyperlink ref="F305" r:id="rId313" xr:uid="{00000000-0004-0000-0000-00003A010000}"/>
+    <hyperlink ref="F306" r:id="rId314" xr:uid="{00000000-0004-0000-0000-00003B010000}"/>
+    <hyperlink ref="F307" r:id="rId315" xr:uid="{00000000-0004-0000-0000-00003C010000}"/>
+    <hyperlink ref="F308" r:id="rId316" xr:uid="{00000000-0004-0000-0000-00003D010000}"/>
+    <hyperlink ref="F309" r:id="rId317" xr:uid="{00000000-0004-0000-0000-00003E010000}"/>
+    <hyperlink ref="F310" r:id="rId318" xr:uid="{00000000-0004-0000-0000-00003F010000}"/>
+    <hyperlink ref="F311" r:id="rId319" xr:uid="{00000000-0004-0000-0000-000040010000}"/>
+    <hyperlink ref="F312" r:id="rId320" xr:uid="{00000000-0004-0000-0000-000041010000}"/>
+    <hyperlink ref="F313" r:id="rId321" xr:uid="{00000000-0004-0000-0000-000042010000}"/>
+    <hyperlink ref="F314" r:id="rId322" xr:uid="{00000000-0004-0000-0000-000043010000}"/>
+    <hyperlink ref="F315" r:id="rId323" xr:uid="{00000000-0004-0000-0000-000044010000}"/>
+    <hyperlink ref="F316" r:id="rId324" xr:uid="{00000000-0004-0000-0000-000045010000}"/>
+    <hyperlink ref="F317" r:id="rId325" xr:uid="{00000000-0004-0000-0000-000046010000}"/>
+    <hyperlink ref="F318" r:id="rId326" xr:uid="{00000000-0004-0000-0000-000047010000}"/>
+    <hyperlink ref="F319" r:id="rId327" xr:uid="{00000000-0004-0000-0000-000048010000}"/>
+    <hyperlink ref="F320" r:id="rId328" xr:uid="{00000000-0004-0000-0000-000049010000}"/>
+    <hyperlink ref="F321" r:id="rId329" xr:uid="{00000000-0004-0000-0000-00004A010000}"/>
+    <hyperlink ref="F322" r:id="rId330" xr:uid="{00000000-0004-0000-0000-00004B010000}"/>
+    <hyperlink ref="F323" r:id="rId331" xr:uid="{00000000-0004-0000-0000-00004C010000}"/>
+    <hyperlink ref="F324" r:id="rId332" xr:uid="{00000000-0004-0000-0000-00004D010000}"/>
+    <hyperlink ref="F325" r:id="rId333" xr:uid="{00000000-0004-0000-0000-00004E010000}"/>
+    <hyperlink ref="F326" r:id="rId334" xr:uid="{00000000-0004-0000-0000-00004F010000}"/>
+    <hyperlink ref="F327" r:id="rId335" xr:uid="{00000000-0004-0000-0000-000050010000}"/>
+    <hyperlink ref="F328" r:id="rId336" xr:uid="{00000000-0004-0000-0000-000051010000}"/>
+    <hyperlink ref="F329" r:id="rId337" xr:uid="{00000000-0004-0000-0000-000052010000}"/>
+    <hyperlink ref="F330" r:id="rId338" xr:uid="{00000000-0004-0000-0000-000053010000}"/>
+    <hyperlink ref="F331" r:id="rId339" xr:uid="{00000000-0004-0000-0000-000054010000}"/>
+    <hyperlink ref="F332" r:id="rId340" xr:uid="{00000000-0004-0000-0000-000055010000}"/>
+    <hyperlink ref="F333" r:id="rId341" xr:uid="{00000000-0004-0000-0000-000056010000}"/>
+    <hyperlink ref="F334" r:id="rId342" xr:uid="{00000000-0004-0000-0000-000057010000}"/>
+    <hyperlink ref="F335" r:id="rId343" xr:uid="{00000000-0004-0000-0000-000058010000}"/>
+    <hyperlink ref="F336" r:id="rId344" xr:uid="{00000000-0004-0000-0000-000059010000}"/>
+    <hyperlink ref="F337" r:id="rId345" xr:uid="{00000000-0004-0000-0000-00005A010000}"/>
+    <hyperlink ref="F338" r:id="rId346" xr:uid="{00000000-0004-0000-0000-00005B010000}"/>
+    <hyperlink ref="F339" r:id="rId347" xr:uid="{00000000-0004-0000-0000-00005C010000}"/>
+    <hyperlink ref="F340" r:id="rId348" xr:uid="{00000000-0004-0000-0000-00005D010000}"/>
+    <hyperlink ref="F341" r:id="rId349" xr:uid="{00000000-0004-0000-0000-00005E010000}"/>
+    <hyperlink ref="F342" r:id="rId350" xr:uid="{00000000-0004-0000-0000-00005F010000}"/>
+    <hyperlink ref="F343" r:id="rId351" xr:uid="{00000000-0004-0000-0000-000060010000}"/>
+    <hyperlink ref="F344" r:id="rId352" xr:uid="{00000000-0004-0000-0000-000061010000}"/>
+    <hyperlink ref="F345" r:id="rId353" xr:uid="{00000000-0004-0000-0000-000062010000}"/>
+    <hyperlink ref="F346" r:id="rId354" xr:uid="{00000000-0004-0000-0000-000063010000}"/>
+    <hyperlink ref="F347" r:id="rId355" xr:uid="{00000000-0004-0000-0000-000064010000}"/>
+    <hyperlink ref="F348" r:id="rId356" xr:uid="{00000000-0004-0000-0000-000065010000}"/>
+    <hyperlink ref="K348" r:id="rId357" xr:uid="{00000000-0004-0000-0000-000066010000}"/>
+    <hyperlink ref="F349" r:id="rId358" xr:uid="{00000000-0004-0000-0000-000067010000}"/>
+    <hyperlink ref="F350" r:id="rId359" xr:uid="{00000000-0004-0000-0000-000068010000}"/>
+    <hyperlink ref="F351" r:id="rId360" xr:uid="{00000000-0004-0000-0000-000069010000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>